<commit_message>
Test monitor now recognising changes to excel and word files
</commit_message>
<xml_diff>
--- a/TestDir/New Microsoft Excel Worksheet.xlsx
+++ b/TestDir/New Microsoft Excel Worksheet.xlsx
@@ -14,9 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>sdlkfjsdlfkj</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>sdflkjsdlfj</t>
+  </si>
+  <si>
+    <t>sldkfjsdlfkdsjf</t>
+  </si>
+  <si>
+    <t>sldkjf</t>
+  </si>
+  <si>
+    <t>sdlfjslfkj</t>
+  </si>
+  <si>
+    <t>sdlkfjslfkj</t>
+  </si>
+  <si>
+    <t>sdlkfsdlfkj</t>
+  </si>
+  <si>
+    <t>sldkfj</t>
+  </si>
+  <si>
+    <t>sldkfdslfkj</t>
+  </si>
+  <si>
+    <t>sdlkfjsdlkfj</t>
+  </si>
+  <si>
+    <t>slkfdslfkj</t>
+  </si>
+  <si>
+    <t>sdlkfsdlkfj</t>
   </si>
 </sst>
 </file>
@@ -358,17 +391,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G7"/>
+  <dimension ref="G2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
+    <row r="2" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
         <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented in dirmonitor but not tested
</commit_message>
<xml_diff>
--- a/TestDir/New Microsoft Excel Worksheet.xlsx
+++ b/TestDir/New Microsoft Excel Worksheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>sdfsdf</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>sdlkfsdlkfj</t>
+  </si>
+  <si>
+    <t>sdlkfjsdlfkj</t>
   </si>
 </sst>
 </file>
@@ -391,15 +394,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G2:L10"/>
+  <dimension ref="D2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:12" x14ac:dyDescent="0.25">
       <c r="I2" t="s">
         <v>7</v>
       </c>
@@ -407,7 +410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>2</v>
       </c>
@@ -415,12 +418,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
       <c r="I5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>8</v>
       </c>
@@ -431,7 +437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
         <v>1</v>
       </c>
@@ -442,7 +448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Working but with exceptions thrown (and null documents created)
</commit_message>
<xml_diff>
--- a/TestDir/New Microsoft Excel Worksheet.xlsx
+++ b/TestDir/New Microsoft Excel Worksheet.xlsx
@@ -14,45 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>sdfsdf</t>
+    <t>sdlkfjsldfkdslkfj</t>
   </si>
   <si>
-    <t>sdflkjsdlfj</t>
-  </si>
-  <si>
-    <t>sldkfjsdlfkdsjf</t>
-  </si>
-  <si>
-    <t>sldkjf</t>
-  </si>
-  <si>
-    <t>sdlfjslfkj</t>
-  </si>
-  <si>
-    <t>sdlkfjslfkj</t>
-  </si>
-  <si>
-    <t>sdlkfsdlfkj</t>
-  </si>
-  <si>
-    <t>sldkfj</t>
-  </si>
-  <si>
-    <t>sldkfdslfkj</t>
-  </si>
-  <si>
-    <t>sdlkfjsdlkfj</t>
-  </si>
-  <si>
-    <t>slkfdslfkj</t>
-  </si>
-  <si>
-    <t>sdlkfsdlkfj</t>
-  </si>
-  <si>
-    <t>sdlkfjsdlfkj</t>
+    <t>sdflksjdflskdjflskdjflskdjfldskjf</t>
   </si>
 </sst>
 </file>
@@ -394,66 +361,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:L10"/>
+  <dimension ref="G3:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
+    <row r="3" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
+    <row r="5" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
         <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>